<commit_message>
readme and tz updated
</commit_message>
<xml_diff>
--- a/tz.xlsx
+++ b/tz.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdgbi\Desktop\S\Vision\predvidenie_vision\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401BF530-E92B-430B-9407-75461D0F0D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="482" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="482"/>
   </bookViews>
   <sheets>
     <sheet name="главная страница" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Промежуток времени</t>
   </si>
@@ -67,12 +61,24 @@
   </si>
   <si>
     <t>Прогноз</t>
+  </si>
+  <si>
+    <t>окружение</t>
+  </si>
+  <si>
+    <t>поведение</t>
+  </si>
+  <si>
+    <t>ценности</t>
+  </si>
+  <si>
+    <t>миссия</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,33 +427,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -458,54 +464,74 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>